<commit_message>
update tagging data - trip 1
</commit_message>
<xml_diff>
--- a/data/taggingData/tagChinData.xlsx
+++ b/data/taggingData/tagChinData.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2047" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2399" uniqueCount="307">
   <si>
     <t>event</t>
   </si>
@@ -544,6 +544,408 @@
   </si>
   <si>
     <t>7696</t>
+  </si>
+  <si>
+    <t>CK10</t>
+  </si>
+  <si>
+    <t>CK11</t>
+  </si>
+  <si>
+    <t>CK12</t>
+  </si>
+  <si>
+    <t>CK13</t>
+  </si>
+  <si>
+    <t>0907</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>0909</t>
+  </si>
+  <si>
+    <t>27-28</t>
+  </si>
+  <si>
+    <t>20015</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>0921</t>
+  </si>
+  <si>
+    <t>0926</t>
+  </si>
+  <si>
+    <t>CF09</t>
+  </si>
+  <si>
+    <t>29-30</t>
+  </si>
+  <si>
+    <t>20027</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>9.0</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>0931</t>
+  </si>
+  <si>
+    <t>0935</t>
+  </si>
+  <si>
+    <t>CF10</t>
+  </si>
+  <si>
+    <t>31-32</t>
+  </si>
+  <si>
+    <t>19980</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>7697</t>
+  </si>
+  <si>
+    <t>7698</t>
+  </si>
+  <si>
+    <t>0943</t>
+  </si>
+  <si>
+    <t>0946</t>
+  </si>
+  <si>
+    <t>33-34</t>
+  </si>
+  <si>
+    <t>20040</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>0950</t>
+  </si>
+  <si>
+    <t>0956</t>
+  </si>
+  <si>
+    <t>CF11</t>
+  </si>
+  <si>
+    <t>35-37</t>
+  </si>
+  <si>
+    <t>20042</t>
+  </si>
+  <si>
+    <t>7699</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>1009</t>
+  </si>
+  <si>
+    <t>1014</t>
+  </si>
+  <si>
+    <t>CF12</t>
+  </si>
+  <si>
+    <t>38-39</t>
+  </si>
+  <si>
+    <t>20025</t>
+  </si>
+  <si>
+    <t>7700</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>1016</t>
+  </si>
+  <si>
+    <t>1021</t>
+  </si>
+  <si>
+    <t>CF13</t>
+  </si>
+  <si>
+    <t>40-41</t>
+  </si>
+  <si>
+    <t>20004</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>7701</t>
+  </si>
+  <si>
+    <t>10.9</t>
+  </si>
+  <si>
+    <t>1028</t>
+  </si>
+  <si>
+    <t>1031</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>19972</t>
+  </si>
+  <si>
+    <t>3.6</t>
+  </si>
+  <si>
+    <t>1036</t>
+  </si>
+  <si>
+    <t>CF14</t>
+  </si>
+  <si>
+    <t>43-44</t>
+  </si>
+  <si>
+    <t>19991</t>
+  </si>
+  <si>
+    <t>7702</t>
+  </si>
+  <si>
+    <t>12.6</t>
+  </si>
+  <si>
+    <t>1038</t>
+  </si>
+  <si>
+    <t>1044</t>
+  </si>
+  <si>
+    <t>45-46</t>
+  </si>
+  <si>
+    <t>20058</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>1132</t>
+  </si>
+  <si>
+    <t>1135</t>
+  </si>
+  <si>
+    <t>20056</t>
+  </si>
+  <si>
+    <t>1137</t>
+  </si>
+  <si>
+    <t>1141</t>
+  </si>
+  <si>
+    <t>CF15</t>
+  </si>
+  <si>
+    <t>20018</t>
+  </si>
+  <si>
+    <t>7703</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1146</t>
+  </si>
+  <si>
+    <t>1151</t>
+  </si>
+  <si>
+    <t>CF16</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>20045</t>
+  </si>
+  <si>
+    <t>7704</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>1155</t>
+  </si>
+  <si>
+    <t>1158</t>
+  </si>
+  <si>
+    <t>8-9</t>
+  </si>
+  <si>
+    <t>19964</t>
+  </si>
+  <si>
+    <t>10-11</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>landed dead</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>12-13</t>
+  </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>CK14</t>
+  </si>
+  <si>
+    <t>CK15</t>
+  </si>
+  <si>
+    <t>CK16</t>
+  </si>
+  <si>
+    <t>CK17</t>
+  </si>
+  <si>
+    <t>CK18</t>
+  </si>
+  <si>
+    <t>CK19</t>
+  </si>
+  <si>
+    <t>CK20</t>
+  </si>
+  <si>
+    <t>CK21</t>
+  </si>
+  <si>
+    <t>CK22</t>
+  </si>
+  <si>
+    <t>CK23</t>
+  </si>
+  <si>
+    <t>CK24</t>
+  </si>
+  <si>
+    <t>CK25</t>
+  </si>
+  <si>
+    <t>CK26</t>
+  </si>
+  <si>
+    <t>CK27</t>
+  </si>
+  <si>
+    <t>CK28</t>
+  </si>
+  <si>
+    <t>CK29</t>
+  </si>
+  <si>
+    <t>CK30</t>
+  </si>
+  <si>
+    <t>1216</t>
+  </si>
+  <si>
+    <t>1221</t>
+  </si>
+  <si>
+    <t>CF17</t>
+  </si>
+  <si>
+    <t>20007</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>7705</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>1224</t>
+  </si>
+  <si>
+    <t>1230</t>
+  </si>
+  <si>
+    <t>CF18</t>
+  </si>
+  <si>
+    <t>19994</t>
+  </si>
+  <si>
+    <t>7706</t>
+  </si>
+  <si>
+    <t>7.5</t>
+  </si>
+  <si>
+    <t>1229</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>19982</t>
+  </si>
+  <si>
+    <t>lots of lice</t>
+  </si>
+  <si>
+    <t>CK31</t>
+  </si>
+  <si>
+    <t>CK32</t>
   </si>
 </sst>
 </file>
@@ -635,13 +1037,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -922,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AD33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AD14" sqref="AD14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,8 +1338,8 @@
     <col min="15" max="15" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12.5546875" style="1" customWidth="1"/>
-    <col min="18" max="22" width="8.88671875" style="1"/>
-    <col min="25" max="29" width="8.88671875" style="11"/>
+    <col min="18" max="23" width="8.88671875" style="1"/>
+    <col min="25" max="29" width="8.88671875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.3">
@@ -1007,25 +1409,25 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AA1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AB1" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AC1" s="9" t="s">
         <v>27</v>
       </c>
       <c r="AD1" t="s">
@@ -1100,25 +1502,25 @@
       <c r="V2" s="1">
         <v>1</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="1">
         <v>10.9</v>
       </c>
       <c r="X2">
         <v>6.3</v>
       </c>
-      <c r="Y2" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="11">
+      <c r="Y2" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1127,7 +1529,7 @@
         <v>89</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B14" si="0">"CT2019"&amp;"_"&amp;C3</f>
+        <f t="shared" ref="B3:B33" si="0">"CT2019"&amp;"_"&amp;C3</f>
         <v>CT2019_002</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -1163,9 +1565,15 @@
       <c r="M3" t="s">
         <v>92</v>
       </c>
+      <c r="N3">
+        <v>11972</v>
+      </c>
       <c r="O3" s="1" t="s">
         <v>93</v>
       </c>
+      <c r="P3" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q3" s="1" t="s">
         <v>94</v>
       </c>
@@ -1184,25 +1592,25 @@
       <c r="V3" s="1">
         <v>1</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="1" t="s">
         <v>96</v>
       </c>
       <c r="X3" t="s">
         <v>96</v>
       </c>
-      <c r="Y3" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="11">
+      <c r="Y3" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="9">
         <v>0</v>
       </c>
       <c r="AD3" t="s">
@@ -1250,9 +1658,15 @@
       <c r="M4" t="s">
         <v>96</v>
       </c>
+      <c r="N4">
+        <v>11972</v>
+      </c>
       <c r="O4" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="P4" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q4" s="1" t="s">
         <v>104</v>
       </c>
@@ -1271,25 +1685,25 @@
       <c r="V4" s="1">
         <v>1</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="X4">
         <v>5.9</v>
       </c>
-      <c r="Y4" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA4" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="11">
+      <c r="Y4" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="9">
         <v>0</v>
       </c>
       <c r="AD4" t="s">
@@ -1337,9 +1751,15 @@
       <c r="M5" t="s">
         <v>109</v>
       </c>
+      <c r="N5">
+        <v>11972</v>
+      </c>
       <c r="O5" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q5" s="1" t="s">
         <v>111</v>
       </c>
@@ -1358,25 +1778,25 @@
       <c r="V5" s="1">
         <v>1</v>
       </c>
-      <c r="W5" t="s">
+      <c r="W5" s="1" t="s">
         <v>96</v>
       </c>
       <c r="X5" t="s">
         <v>96</v>
       </c>
-      <c r="Y5" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="11">
+      <c r="Y5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="9">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
@@ -1451,25 +1871,25 @@
       <c r="V6" s="1">
         <v>0</v>
       </c>
-      <c r="W6" t="s">
+      <c r="W6" s="1" t="s">
         <v>96</v>
       </c>
       <c r="X6" t="s">
         <v>96</v>
       </c>
-      <c r="Y6" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="11">
+      <c r="Y6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="9">
         <v>0</v>
       </c>
       <c r="AD6" t="s">
@@ -1517,9 +1937,15 @@
       <c r="M7" t="s">
         <v>120</v>
       </c>
+      <c r="N7">
+        <v>11972</v>
+      </c>
       <c r="O7" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q7" s="1" t="s">
         <v>122</v>
       </c>
@@ -1538,25 +1964,25 @@
       <c r="V7" s="1">
         <v>1</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="1">
         <v>10.6</v>
       </c>
       <c r="X7">
         <v>7.7</v>
       </c>
-      <c r="Y7" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="11">
+      <c r="Y7" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1607,6 +2033,9 @@
       <c r="O8" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q8" s="1" t="s">
         <v>127</v>
       </c>
@@ -1625,25 +2054,25 @@
       <c r="V8" s="1">
         <v>0</v>
       </c>
-      <c r="W8" t="s">
+      <c r="W8" s="1" t="s">
         <v>96</v>
       </c>
       <c r="X8" t="s">
         <v>96</v>
       </c>
-      <c r="Y8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="11">
+      <c r="Y8" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1688,9 +2117,15 @@
       <c r="M9" t="s">
         <v>133</v>
       </c>
+      <c r="N9">
+        <v>11972</v>
+      </c>
       <c r="O9" s="1" t="s">
         <v>134</v>
       </c>
+      <c r="P9" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q9" s="1" t="s">
         <v>135</v>
       </c>
@@ -1709,25 +2144,25 @@
       <c r="V9" s="1">
         <v>1</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="1">
         <v>8.1999999999999993</v>
       </c>
       <c r="X9">
         <v>4.4000000000000004</v>
       </c>
-      <c r="Y9" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="11">
+      <c r="Y9" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1772,9 +2207,15 @@
       <c r="M10" t="s">
         <v>96</v>
       </c>
+      <c r="N10">
+        <v>11972</v>
+      </c>
       <c r="O10" s="1" t="s">
         <v>138</v>
       </c>
+      <c r="P10" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q10" s="1" t="s">
         <v>139</v>
       </c>
@@ -1793,29 +2234,32 @@
       <c r="V10" s="1">
         <v>1</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="1">
         <v>6.5</v>
       </c>
       <c r="X10">
         <v>5.6</v>
       </c>
-      <c r="Y10" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="11">
+      <c r="Y10" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_016</v>
@@ -1853,9 +2297,15 @@
       <c r="M11" t="s">
         <v>150</v>
       </c>
+      <c r="N11">
+        <v>11972</v>
+      </c>
       <c r="O11" s="1" t="s">
         <v>151</v>
       </c>
+      <c r="P11" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q11" s="1" t="s">
         <v>152</v>
       </c>
@@ -1874,29 +2324,32 @@
       <c r="V11" s="1">
         <v>1</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="1">
         <v>6.2</v>
       </c>
       <c r="X11">
         <v>1.4</v>
       </c>
-      <c r="Y11" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="11">
+      <c r="Y11" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>174</v>
+      </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_016</v>
@@ -1934,9 +2387,15 @@
       <c r="M12" t="s">
         <v>155</v>
       </c>
+      <c r="N12">
+        <v>11972</v>
+      </c>
       <c r="O12" s="1" t="s">
         <v>156</v>
       </c>
+      <c r="P12" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q12" s="1" t="s">
         <v>157</v>
       </c>
@@ -1955,25 +2414,25 @@
       <c r="V12" s="1">
         <v>1</v>
       </c>
-      <c r="W12" t="s">
+      <c r="W12" s="1" t="s">
         <v>96</v>
       </c>
       <c r="X12" t="s">
         <v>96</v>
       </c>
-      <c r="Y12" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC12" s="11">
+      <c r="Y12" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="9">
         <v>0</v>
       </c>
       <c r="AD12" t="s">
@@ -1981,6 +2440,9 @@
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>175</v>
+      </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_017</v>
@@ -2018,9 +2480,15 @@
       <c r="M13" t="s">
         <v>96</v>
       </c>
+      <c r="N13">
+        <v>11972</v>
+      </c>
       <c r="O13" s="1" t="s">
         <v>161</v>
       </c>
+      <c r="P13" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q13" s="1" t="s">
         <v>162</v>
       </c>
@@ -2045,19 +2513,19 @@
       <c r="X13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Y13" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="11">
+      <c r="Y13" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="9">
         <v>0</v>
       </c>
       <c r="AD13" t="s">
@@ -2065,6 +2533,9 @@
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>176</v>
+      </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>CT2019_017</v>
@@ -2102,9 +2573,15 @@
       <c r="M14" t="s">
         <v>167</v>
       </c>
+      <c r="N14">
+        <v>11972</v>
+      </c>
       <c r="O14" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="P14" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="Q14" s="1" t="s">
         <v>169</v>
       </c>
@@ -2129,23 +2606,1727 @@
       <c r="X14" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="Y14" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="11">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="11">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="11">
-        <v>0</v>
-      </c>
-      <c r="AC14" s="11">
+      <c r="Y14" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="9">
         <v>0</v>
       </c>
       <c r="AD14" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>271</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_019</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H15">
+        <v>61</v>
+      </c>
+      <c r="I15">
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K15" t="s">
+        <v>132</v>
+      </c>
+      <c r="L15">
+        <v>414</v>
+      </c>
+      <c r="M15" t="s">
+        <v>96</v>
+      </c>
+      <c r="N15">
+        <v>11972</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V15" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y15" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_019</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F16">
+        <v>22</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16">
+        <v>67</v>
+      </c>
+      <c r="I16">
+        <v>40</v>
+      </c>
+      <c r="J16" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16">
+        <v>415</v>
+      </c>
+      <c r="M16" t="s">
+        <v>186</v>
+      </c>
+      <c r="N16">
+        <v>11972</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q16" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="X16">
+        <v>3.1</v>
+      </c>
+      <c r="Y16" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>273</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_020</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="F17">
+        <v>26</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H17">
+        <v>80</v>
+      </c>
+      <c r="I17">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17">
+        <v>416</v>
+      </c>
+      <c r="M17" t="s">
+        <v>194</v>
+      </c>
+      <c r="N17">
+        <v>11972</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q17" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="X17">
+        <v>5.8</v>
+      </c>
+      <c r="Y17" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>274</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_020</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F18">
+        <v>28</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18">
+        <v>56</v>
+      </c>
+      <c r="I18">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" t="s">
+        <v>78</v>
+      </c>
+      <c r="L18">
+        <v>417</v>
+      </c>
+      <c r="M18" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18">
+        <v>11972</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="X18">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Y18" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19">
+        <v>26</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19">
+        <v>59</v>
+      </c>
+      <c r="I19">
+        <v>38</v>
+      </c>
+      <c r="J19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19">
+        <v>418</v>
+      </c>
+      <c r="M19" t="s">
+        <v>208</v>
+      </c>
+      <c r="N19">
+        <v>11972</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="X19">
+        <v>1.8</v>
+      </c>
+      <c r="Y19" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB19" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>276</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="F20">
+        <v>26</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H20">
+        <v>73</v>
+      </c>
+      <c r="I20">
+        <v>47</v>
+      </c>
+      <c r="J20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L20">
+        <v>419</v>
+      </c>
+      <c r="M20" t="s">
+        <v>215</v>
+      </c>
+      <c r="N20">
+        <v>11972</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="X20">
+        <v>2.4</v>
+      </c>
+      <c r="Y20" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB20" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>277</v>
+      </c>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F21">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21">
+        <v>78</v>
+      </c>
+      <c r="I21">
+        <v>45</v>
+      </c>
+      <c r="J21" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21">
+        <v>420</v>
+      </c>
+      <c r="M21" t="s">
+        <v>222</v>
+      </c>
+      <c r="N21">
+        <v>11972</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q21" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="X21">
+        <v>7.6</v>
+      </c>
+      <c r="Y21" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB21" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>278</v>
+      </c>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F22">
+        <v>16</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H22">
+        <v>65</v>
+      </c>
+      <c r="I22">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
+        <v>77</v>
+      </c>
+      <c r="K22" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22">
+        <v>421</v>
+      </c>
+      <c r="M22" t="s">
+        <v>96</v>
+      </c>
+      <c r="N22">
+        <v>11972</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V22" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W22" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="X22">
+        <v>1.5</v>
+      </c>
+      <c r="Y22" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>279</v>
+      </c>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="F23">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H23">
+        <v>77</v>
+      </c>
+      <c r="I23">
+        <v>46</v>
+      </c>
+      <c r="J23" t="s">
+        <v>77</v>
+      </c>
+      <c r="K23" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23">
+        <v>422</v>
+      </c>
+      <c r="M23" t="s">
+        <v>234</v>
+      </c>
+      <c r="N23">
+        <v>11972</v>
+      </c>
+      <c r="O23" t="s">
+        <v>235</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="S23" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W23" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="X23">
+        <v>7.2</v>
+      </c>
+      <c r="Y23" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>280</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_021</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F24">
+        <v>22</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H24">
+        <v>70</v>
+      </c>
+      <c r="I24">
+        <v>43</v>
+      </c>
+      <c r="J24" t="s">
+        <v>77</v>
+      </c>
+      <c r="K24" t="s">
+        <v>78</v>
+      </c>
+      <c r="L24">
+        <v>423</v>
+      </c>
+      <c r="M24" t="s">
+        <v>96</v>
+      </c>
+      <c r="N24">
+        <v>11972</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="X24">
+        <v>3.2</v>
+      </c>
+      <c r="Y24" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>281</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_022</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F25">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25">
+        <v>54</v>
+      </c>
+      <c r="I25">
+        <v>33</v>
+      </c>
+      <c r="J25" t="s">
+        <v>77</v>
+      </c>
+      <c r="K25" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25">
+        <v>424</v>
+      </c>
+      <c r="M25" t="s">
+        <v>96</v>
+      </c>
+      <c r="N25">
+        <v>15631</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W25" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="X25">
+        <v>1.5</v>
+      </c>
+      <c r="Y25" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>282</v>
+      </c>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_022</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="F26">
+        <v>24</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H26">
+        <v>64</v>
+      </c>
+      <c r="I26">
+        <v>39</v>
+      </c>
+      <c r="J26" t="s">
+        <v>77</v>
+      </c>
+      <c r="K26" t="s">
+        <v>78</v>
+      </c>
+      <c r="L26">
+        <v>425</v>
+      </c>
+      <c r="M26" t="s">
+        <v>250</v>
+      </c>
+      <c r="N26">
+        <v>15631</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W26" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="X26">
+        <v>1.4</v>
+      </c>
+      <c r="Y26" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_022</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F27">
+        <v>16</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H27">
+        <v>72</v>
+      </c>
+      <c r="I27">
+        <v>46</v>
+      </c>
+      <c r="J27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27">
+        <v>426</v>
+      </c>
+      <c r="M27" t="s">
+        <v>256</v>
+      </c>
+      <c r="N27">
+        <v>15631</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="U27" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W27" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="X27">
+        <v>4.3</v>
+      </c>
+      <c r="Y27" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>284</v>
+      </c>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_022</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="F28">
+        <v>30</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28">
+        <v>59</v>
+      </c>
+      <c r="I28">
+        <v>35</v>
+      </c>
+      <c r="J28" t="s">
+        <v>77</v>
+      </c>
+      <c r="K28" t="s">
+        <v>78</v>
+      </c>
+      <c r="L28">
+        <v>427</v>
+      </c>
+      <c r="M28" t="s">
+        <v>96</v>
+      </c>
+      <c r="N28">
+        <v>15631</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="P28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q28" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U28" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="W28" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="X28">
+        <v>3.4</v>
+      </c>
+      <c r="Y28" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>285</v>
+      </c>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_022</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29">
+        <v>53</v>
+      </c>
+      <c r="I29">
+        <v>30</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L29">
+        <v>428</v>
+      </c>
+      <c r="M29" t="s">
+        <v>96</v>
+      </c>
+      <c r="N29">
+        <v>15631</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="X29">
+        <v>1.5</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>286</v>
+      </c>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_023</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H30">
+        <v>54</v>
+      </c>
+      <c r="I30">
+        <v>31</v>
+      </c>
+      <c r="J30" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" t="s">
+        <v>78</v>
+      </c>
+      <c r="L30">
+        <v>429</v>
+      </c>
+      <c r="M30" t="s">
+        <v>96</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="X30">
+        <v>0.7</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>287</v>
+      </c>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_023</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F31">
+        <v>30</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H31">
+        <v>68</v>
+      </c>
+      <c r="I31">
+        <v>42</v>
+      </c>
+      <c r="J31" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31">
+        <v>430</v>
+      </c>
+      <c r="M31" t="s">
+        <v>290</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="X31">
+        <v>4.3</v>
+      </c>
+      <c r="Y31" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>305</v>
+      </c>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_023</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F32">
+        <v>18</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H32">
+        <v>71</v>
+      </c>
+      <c r="I32">
+        <v>48</v>
+      </c>
+      <c r="J32" t="s">
+        <v>77</v>
+      </c>
+      <c r="K32" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32">
+        <v>431</v>
+      </c>
+      <c r="M32" t="s">
+        <v>297</v>
+      </c>
+      <c r="O32" t="s">
+        <v>138</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="S32" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="T32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U32" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W32" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="X32">
+        <v>4.5</v>
+      </c>
+      <c r="Y32" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>306</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>CT2019_023</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F33">
+        <v>18</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33">
+        <v>71</v>
+      </c>
+      <c r="I33">
+        <v>43</v>
+      </c>
+      <c r="J33" t="s">
+        <v>77</v>
+      </c>
+      <c r="K33" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33">
+        <v>432</v>
+      </c>
+      <c r="M33" t="s">
+        <v>96</v>
+      </c>
+      <c r="O33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q33" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="R33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="S33" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="T33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="U33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V33" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W33" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="X33">
+        <v>3.9</v>
+      </c>
+      <c r="Y33" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="9">
+        <v>0</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -2184,20 +4365,20 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="10" t="s">
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9" t="s">
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="S1" s="9"/>
+      <c r="S1" s="10"/>
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
     </row>
@@ -2345,11 +4526,11 @@
       <c r="B9" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">

</xml_diff>

<commit_message>
finish trip 4 data
</commit_message>
<xml_diff>
--- a/data/taggingData/tagChinData.xlsx
+++ b/data/taggingData/tagChinData.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6120" uniqueCount="1419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6139" uniqueCount="1427">
   <si>
     <t>event</t>
   </si>
@@ -4280,6 +4280,30 @@
   </si>
   <si>
     <t>8.7</t>
+  </si>
+  <si>
+    <t>CK230</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>1456</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>CF88</t>
+  </si>
+  <si>
+    <t>19861</t>
+  </si>
+  <si>
+    <t>089</t>
+  </si>
+  <si>
+    <t>8197</t>
   </si>
 </sst>
 </file>
@@ -4381,8 +4405,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4568,7 +4594,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4651,6 +4677,7 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4733,6 +4760,7 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5011,11 +5039,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD230"/>
+  <dimension ref="A1:AD231"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="O1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AD216" sqref="AD216"/>
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AD231" sqref="AD231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -20011,7 +20039,7 @@
         <v>797</v>
       </c>
       <c r="B166" t="str">
-        <f t="shared" ref="B166:B230" si="3">"CT2019"&amp;"_"&amp;C166</f>
+        <f t="shared" ref="B166:B231" si="3">"CT2019"&amp;"_"&amp;C166</f>
         <v>CT2019_120</v>
       </c>
       <c r="C166" s="1" t="s">
@@ -25895,6 +25923,96 @@
         <v>0</v>
       </c>
       <c r="AC230" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:29">
+      <c r="A231" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B231" t="str">
+        <f t="shared" si="3"/>
+        <v>CT2019_186</v>
+      </c>
+      <c r="C231" s="1" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D231" s="1" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E231" s="1" t="s">
+        <v>1422</v>
+      </c>
+      <c r="F231">
+        <v>24</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H231">
+        <v>83</v>
+      </c>
+      <c r="I231">
+        <v>48</v>
+      </c>
+      <c r="J231" t="s">
+        <v>77</v>
+      </c>
+      <c r="K231" t="s">
+        <v>78</v>
+      </c>
+      <c r="L231">
+        <v>841</v>
+      </c>
+      <c r="M231" t="s">
+        <v>1423</v>
+      </c>
+      <c r="N231" s="1" t="s">
+        <v>1395</v>
+      </c>
+      <c r="O231" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="P231" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q231" s="1" t="s">
+        <v>1424</v>
+      </c>
+      <c r="R231" s="1" t="s">
+        <v>1425</v>
+      </c>
+      <c r="S231" s="1" t="s">
+        <v>1426</v>
+      </c>
+      <c r="T231" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="U231" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="V231" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="W231" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="X231" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="Y231" s="9">
+        <v>0</v>
+      </c>
+      <c r="Z231" s="9">
+        <v>0</v>
+      </c>
+      <c r="AA231" s="9">
+        <v>0</v>
+      </c>
+      <c r="AB231" s="9">
+        <v>0</v>
+      </c>
+      <c r="AC231" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
debug data and create trimmed file for K. Pellett
</commit_message>
<xml_diff>
--- a/data/taggingData/tagChinData.xlsx
+++ b/data/taggingData/tagChinData.xlsx
@@ -5736,7 +5736,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -5771,7 +5771,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -5958,9 +5958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N241" sqref="N241"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P287" sqref="P287"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31883,7 +31883,7 @@
         <v>1234</v>
       </c>
       <c r="P286" s="10" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="Q286" s="1" t="s">
         <v>96</v>

</xml_diff>

<commit_message>
update tagging data w/ pit codes
</commit_message>
<xml_diff>
--- a/data/taggingData/tagChinData.xlsx
+++ b/data/taggingData/tagChinData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7358" uniqueCount="1671">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7360" uniqueCount="1673">
   <si>
     <t>event</t>
   </si>
@@ -5041,6 +5041,12 @@
   </si>
   <si>
     <t>face wound</t>
+  </si>
+  <si>
+    <t>RECPATURED (see file)</t>
+  </si>
+  <si>
+    <t>RECAPTURED (see file)</t>
   </si>
 </sst>
 </file>
@@ -5958,9 +5964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD294"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A269" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P287" sqref="P287"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9026,7 +9032,7 @@
         <v>310</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>96</v>
@@ -11068,6 +11074,9 @@
       <c r="AC56" s="9">
         <v>0</v>
       </c>
+      <c r="AD56" t="s">
+        <v>1671</v>
+      </c>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
@@ -14880,6 +14889,9 @@
       </c>
       <c r="AC98" s="9">
         <v>0</v>
+      </c>
+      <c r="AD98" t="s">
+        <v>1672</v>
       </c>
     </row>
     <row r="99" spans="1:30" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update w/ tag recoveries
</commit_message>
<xml_diff>
--- a/data/taggingData/tagChinData.xlsx
+++ b/data/taggingData/tagChinData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7362" uniqueCount="1673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7366" uniqueCount="1673">
   <si>
     <t>event</t>
   </si>
@@ -5964,9 +5964,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD294"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N119" sqref="N119"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6163,6 +6163,9 @@
       <c r="AC2" s="9">
         <v>0</v>
       </c>
+      <c r="AD2" t="s">
+        <v>1672</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -11977,6 +11980,9 @@
       <c r="AC66" s="9">
         <v>0</v>
       </c>
+      <c r="AD66" t="s">
+        <v>1671</v>
+      </c>
     </row>
     <row r="67" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
@@ -24505,6 +24511,9 @@
       <c r="AC204" s="9">
         <v>0</v>
       </c>
+      <c r="AD204" t="s">
+        <v>1672</v>
+      </c>
     </row>
     <row r="205" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
@@ -29847,6 +29856,9 @@
       </c>
       <c r="AC263" s="9">
         <v>0</v>
+      </c>
+      <c r="AD263" t="s">
+        <v>1672</v>
       </c>
     </row>
     <row r="264" spans="1:30" x14ac:dyDescent="0.3">

</xml_diff>